<commit_message>
physics 3.06, 3.07 final
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/Physics/lab_3_06/3.06.xlsx
+++ b/2COURSE/2SEM/Physics/lab_3_06/3.06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\Physics\lab_3_06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1D0A4D-E057-4EFD-9B0A-C06079045CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8C1D59-7218-4FF3-BC70-D7BAD76010D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>R1,Ом</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>&lt;- откуда это и используется ли где?</t>
   </si>
 </sst>
 </file>
@@ -377,6 +374,12 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,12 +400,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,7 +672,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10034949686143989"/>
-          <c:y val="7.3671662481172476E-2"/>
+          <c:y val="4.6220680676274023E-2"/>
           <c:w val="0.81295607765615097"/>
           <c:h val="0.83458874142291917"/>
         </c:manualLayout>
@@ -975,15 +972,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>570807</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>93518</xdr:rowOff>
+      <xdr:colOff>581693</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>231370</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>93518</xdr:rowOff>
+      <xdr:colOff>242256</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1406,7 +1403,7 @@
   <dimension ref="A1:AB56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1437,30 +1434,30 @@
         <v>4700</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="31"/>
-      <c r="P2" s="32" t="s">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="35"/>
+      <c r="P2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="32"/>
+      <c r="Q2" s="36"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="32"/>
+      <c r="T2" s="36"/>
       <c r="U2" s="11"/>
-      <c r="V2" s="33" t="s">
+      <c r="V2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="32"/>
+      <c r="W2" s="36"/>
       <c r="X2" s="11"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -2045,11 +2042,11 @@
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
       <c r="F12" s="2">
         <v>9</v>
       </c>
@@ -2112,11 +2109,11 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
       <c r="F13" s="2">
         <v>10</v>
       </c>
@@ -2506,10 +2503,10 @@
         <f>SQRT((0.05/1.7)^2+(0.1)^2)*100</f>
         <v>10.423555968629032</v>
       </c>
-      <c r="T19" s="34"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2519,14 +2516,14 @@
         <f>B18*B19/100</f>
         <v>33251.143539926612</v>
       </c>
-      <c r="T20" s="34"/>
-      <c r="U20" s="36" t="s">
+      <c r="T20" s="27"/>
+      <c r="U20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="V20" s="35">
+      <c r="V20" s="28">
         <v>1929</v>
       </c>
-      <c r="W20" s="35"/>
+      <c r="W20" s="28"/>
       <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
@@ -2541,15 +2538,15 @@
         <f>5*0.8*B5/B7</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="T21" s="34"/>
-      <c r="U21" s="35" t="s">
+      <c r="T21" s="27"/>
+      <c r="U21" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="V21" s="35">
+      <c r="V21" s="28">
         <f>AVERAGE(V4:V18)</f>
         <v>25.816321542480303</v>
       </c>
-      <c r="W21" s="35"/>
+      <c r="W21" s="28"/>
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="11"/>
@@ -2564,15 +2561,15 @@
         <f>((0.05/0.5)^2+(0.1)^2+(0.1)^2)^(1/2)*100</f>
         <v>17.320508075688775</v>
       </c>
-      <c r="T22" s="34"/>
-      <c r="U22" s="36" t="s">
+      <c r="T22" s="27"/>
+      <c r="U22" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="V22" s="35">
+      <c r="V22" s="28">
         <f>V21*V20/100</f>
         <v>497.99684255444504</v>
       </c>
-      <c r="W22" s="35"/>
+      <c r="W22" s="28"/>
       <c r="X22" s="11"/>
       <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
@@ -2587,14 +2584,12 @@
         <f>B21*B22/100</f>
         <v>1.385640646055102E-3</v>
       </c>
-      <c r="T23" s="34"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
       <c r="X23" s="11"/>
-      <c r="Y23" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
       <c r="AA23" s="11"/>
       <c r="AB23" s="11"/>
@@ -2607,10 +2602,10 @@
         <f>5*3.3*B5/B7</f>
         <v>3.2999999999999995E-2</v>
       </c>
-      <c r="T24" s="34"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
       <c r="X24" s="11"/>
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
@@ -2625,14 +2620,14 @@
         <f>((0.05/1.6)^2+(0.1)^2+(0.1)^2+(0.1/5)^2)^(1/2)*100</f>
         <v>14.620725871173429</v>
       </c>
-      <c r="T25" s="34"/>
-      <c r="U25" s="36" t="s">
+      <c r="T25" s="27"/>
+      <c r="U25" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="V25" s="35">
+      <c r="V25" s="28">
         <v>9850</v>
       </c>
-      <c r="W25" s="35"/>
+      <c r="W25" s="28"/>
       <c r="X25" s="11"/>
       <c r="Y25" s="11"/>
       <c r="Z25" s="11"/>
@@ -2652,15 +2647,15 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="37" t="s">
+      <c r="T26" s="27"/>
+      <c r="U26" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="V26" s="35">
+      <c r="V26" s="28">
         <f>V4</f>
         <v>22.053630065699803</v>
       </c>
-      <c r="W26" s="35"/>
+      <c r="W26" s="28"/>
       <c r="X26" s="11"/>
       <c r="Y26" s="11"/>
       <c r="Z26" s="11"/>
@@ -2675,15 +2670,15 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="37" t="s">
+      <c r="T27" s="27"/>
+      <c r="U27" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="V27" s="35">
+      <c r="V27" s="28">
         <f>W4</f>
         <v>2574.9548609441658</v>
       </c>
-      <c r="W27" s="35"/>
+      <c r="W27" s="28"/>
       <c r="X27" s="11"/>
       <c r="Y27" s="11"/>
       <c r="Z27" s="11"/>
@@ -2703,10 +2698,10 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="28"/>
       <c r="X28" s="11"/>
       <c r="Y28" s="11"/>
       <c r="Z28" s="11"/>
@@ -2721,14 +2716,14 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="35" t="s">
+      <c r="T29" s="27"/>
+      <c r="U29" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="V29" s="35">
+      <c r="V29" s="28">
         <v>319000</v>
       </c>
-      <c r="W29" s="35"/>
+      <c r="W29" s="28"/>
       <c r="X29" s="11"/>
       <c r="Y29" s="11"/>
       <c r="Z29" s="11"/>
@@ -2747,10 +2742,10 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
       <c r="X30" s="11"/>
       <c r="Y30" s="11"/>
       <c r="Z30" s="11"/>

</xml_diff>

<commit_message>
physics 3.06, 3.07 final release
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/Physics/lab_3_06/3.06.xlsx
+++ b/2COURSE/2SEM/Physics/lab_3_06/3.06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\Physics\lab_3_06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8C1D59-7218-4FF3-BC70-D7BAD76010D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E588E4-EEE9-4F7C-846A-78E655047452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,6 +613,44 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Напряженность электриеского поля </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>E, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>В/м</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -629,6 +667,46 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Электрическая</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> смещенность </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>D, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t>Кл/м</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>^2</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -671,8 +749,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10034949686143989"/>
-          <c:y val="4.6220680676274023E-2"/>
+          <c:x val="0.10034954182863064"/>
+          <c:y val="5.1726597152765411E-2"/>
           <c:w val="0.81295607765615097"/>
           <c:h val="0.83458874142291917"/>
         </c:manualLayout>
@@ -930,6 +1008,32 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Напряженность электриеского поля </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>E, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>В/м</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -946,6 +1050,29 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Диэлектрическая</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> проницаемость</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -971,16 +1098,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581693</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28205</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>531033</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>182218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>242256</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28205</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>597765</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>168966</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1009,16 +1136,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>290944</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>11775</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>557064</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>595745</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>11775</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>13124</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>178906</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1403,7 +1530,7 @@
   <dimension ref="A1:AB56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>